<commit_message>
Adding GeneratePdf Feature and PDF Template
</commit_message>
<xml_diff>
--- a/app/database/question_bank.xlsx
+++ b/app/database/question_bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,7 +700,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Changing of atoms of one element iinto those of another element to form new products</t>
+          <t>Changing of the atoms of one element into those of another element to form new products</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Reactants are in a gaseous state</t>
+          <t>Reactants are in gaseous state</t>
         </is>
       </c>
     </row>
@@ -1043,12 +1043,1988 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Methyl orange is </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Pink in acidic medium and yellow in basic medium, Yellow in acidic medium and pink in basic medium, Colourless in acidic medium and pink in basic medium, Pink in acidic medium and colorless in basic medium</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Pink in acidic medium and yellow in basic medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lime water is </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CaO, Ca(OH)2, CaCo3, CaCl2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ca(OH)2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Which of the following salts has no water of crystallization ?</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Blue Vitrol, Washing Soda, Baking Soda, Gypsum</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Baking Soda</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Most of the oxides of metals when react with acid , form ___</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>A Base, An Acid, A Salt, Either (1) or (2)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>A Salt</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Generally, when certain metals react with an acid they release ___ gas.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Nitrogen, Oxygen, Hydrogen, Argon</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Which of the given is a strong base ?</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Calcium Hydroxide, Magnesium Hydroxide, Ammonium Hydroxide, Potassium Hydroxide</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Potassium Hydroxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Which one of the given is the PH value of pure water</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0, 7, 8, 1</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Which one of the following  is formed when calcium hydroxide reacts with carbon dioxide ?</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Hydrogen gas, Water, Salt, Both Water and Salt</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Both Water and Salt</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>When acids dissolve in water it releases ___.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>H+ ion, H- ion, H30+ ion, H302+ ion</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>H30+ ion</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Black ash is ___.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Dry KOH, Barium sulphate, Charcoal, Hydrated KOH</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Barium sulphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>The pH of commonly used toothpaste is ?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>&lt;6.5, ≥ 7, ≥ 2.2, None of these</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>≥ 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The pH of Gastric juice is </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>&lt;6.5, ≥ 7, 1.5 to 3.5, None of Above</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1.5 to 3.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>The chemical formula of Plaster of Paris is</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CaSo4, 1/2 H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>What happens when a solution of an acid is mixed with a solution of base in a test tube ?
+i) The temperature of the solution increases.
+ii) The temperature of the solution decreases.
+iii) The temperature of the solution remains the same.
+iv) Salt formation takes place.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>(i) only, (i) and (ii), (ii) and (iii), (i) and (iv)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>(i) and (iv)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chemical formula of washing soda is </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Na2Co3, 10H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>An aqueous solution turns red litmus solution blue. Excess addition of which of the following solution would be the reverse change ?</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Baking Powder, Lime, Ammonium hydroxide solution, Hydrochloric acid</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Hydrochloric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sodium Hydroxide is used </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>as an antacid, in manufacturing of soap, as a cleansing agent, in alkaline</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>in alkaline</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>The pH of a solution is 7. How can you increase its pH ?</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>By adding a small amount of acid, By adding small amount of base, By adding a small amount of salt, By passing carbon dioxide gas through it</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>By adding small amount of base</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Sodium hydroxide is a ____</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>weak base, weak acid, strong base, strong acid</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>strong base</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Which of the following gives the correct increasing order of acidic strength ?</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Water &lt; Acetic acid &lt; Hydrochloric acid, Water &lt; Hydrochloric acid &lt; Acetic acid, Acetic acid &lt; Water &lt; Hydrochloric acid, Hydrochloric acid &lt; Water &lt; Acetic acid</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Water &lt; Acetic acid &lt; Hydrochloric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Rain is called acid rain when its</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>pH falls below 7, pH falls below 6, pH falls below 5.6, pH is above 7</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>pH falls below 5.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>If a few drops of a concentrated acid accidentally spills over the hand of the student, what should be done ?</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Wash the hand with saline water, Wash the hand immediately with plenty of water and apply a paste of sodium hydrogencarbonate, After washing with plenty of water apply solution of sodium hydroxide on the hand., Neutralize the acid with a strong alkali</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Neutralize the acid with strong alkali</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Farmers neutralize the effect of acidity of the soil by adding </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Slaked lime, gypsum, caustic soda, baking soda</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Slaked lime</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>What is the pH range of our body ?</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>7.0 - 7.8, 7.2 - 8.0, 7.0 - 8.4, 7.2 - 8.4</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>7.0 - 7.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Tooth enamel is made up of ?</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>calcium phosphate, calcium carbonate, calcium oxide, potassium</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>calcium phosphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Increase in the OH- ion concentration, leads to</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>an increase in the pH of solution, a decrease in the pH of solution, doesn't alter the pH of solution, decrease the basic strength of the solution.</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>an increase in the pH of solution</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Lime water reacts with chlorine to give</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>bleaching powder, baking powder, baking soda, washing soda</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>bleaching powder</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Alkalis are</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>acids (which are soluble in water), acids (which are insoluble in water), bases (which are soluble in water), bases (which are insoluble in water)</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>bases (which are soluble in water)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Acids react with metal carbonates to liberate ___ gas</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Carbon dioxide, Carbon monoxide, hydrogen, water</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Carbon monoxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Lime water turns milky when carbon dioxide is passed due to formation of ___.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>CaCO3, CaO, CO2, CaSo4</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>CaCO3</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How is the concentration of hydronium ions (H30+) affected when a solution of an acid is diluted </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Increases, Decreases, Remains same, Becomes Zero</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Decreases</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>From the following, which one is the example of chemical reaction ?</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Grapes get fermented, Breakdown of food, Formation of curd, All of the above</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>All of the above</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Which of the following shows an oxidation reaction ?</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Gain of Oxygen, Loss of Oxygen, Gain of Hydrogen, None of Above</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Gain of Oxygen</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>What is the product obtained when lead nitrate is heated ?</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Lead Oxide, Lead Nitrate, Lead Sulphate, Lead Chloride</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Lead Oxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>In a chemical equation, the number written in front of a chemical formula represents:</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Atomic Number, Molecular Mass, Number of Molecules, Number of atoms or molecules taking part in the reaction</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Number of Molecules</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>The balanced chemical equation for the reaction between hydrogen and oxygen to form water is:</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>H2 + O2 -&gt; H20, 2H2 + O2 -&gt; 2H20,  H20 -&gt; H2 + O2, 2H2O -&gt; 2H2 + O2</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2H2 + O2 -&gt; 2H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>The type of chemical reaction in which two or more substances combine to form a single product is called</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Combination Reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>What is the product obtained when copper (II) oxide is heated with hydrogen gas ?</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Copper Oxide, Copper Metal, Copper Sulphate, Copper Chloride</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Copper Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Which of the following statements is true regarding a decomposition reaction</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>A single reactant breaks down into two or more products, Two or more reactants combine to form a single product, A metal displaces another metal to form its salt solution, A non metal displaces another non-metal from its compound.</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>A single reactant breaks down into two or more products</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The chemical name of the baking soda commonly used in cooking is </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Sodium chloride, Sodium bicarbonate, Sodium carbonate, sodium hydroxide</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Sodium bicarbonate</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>The chemical formula for sulfuric acid is:</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>H2SO3, HCL, H2SO4, HNO3</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>H2SO4</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Reaction of 'magnesium' with air is</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Exothermic reaction, Endothermic reaction, Reversible reaction, Substitution</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Exothermic reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>What chemicals are used in fireworks</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Copper Chloride, Calcium Chloride, Barium Chloride, All of Above</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>All of Above</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>When crystals of lead nitrate are heated strongly in a dry test tube</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Crystals immediately melt, Brown residue is left, White fumes appear in the tube, A yellow residue is left</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Brown residue is left</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The reaction in which two compounds exchange their ions to form two new compounds is called </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Double displacement reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Which of the following is characteristics of acids ?</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Sour Taste, Bitter Taste, Slippery feel, Blue litmus to Red</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Sour Taste</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Which of the following is a weak base ?</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Sodium hydroxide, Ammonium Hydroxide, Calcium Hydroxide, Potassium Hydroxide</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Ammonium Hydroxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Which of the following is an example of salt ?</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Sugar, Calcium Carbonate, Sodium Chloride, Hydrogen Peroxide</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Sodium Chloride</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>What is the chemical formula of hydrochloric acid is HCL ?</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>True/False</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Which of the following is natural indicator ?</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Phenolphthalein, Methyl Orange, Litmus, Vitrol Blue</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Litmus</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Which acid is found in vinegar ?</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Sulfuric Acid, Nitric Acid, Acetic Acid, HCL</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Acetic Acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>What is the pH value of lemon juice ?</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1, 7, 14, 5</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Which of the following is a weak acid ?</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>HCL, Sulfuric acid, Nitric Acid, Carbonic Acid</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Carbonic Acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>What is the chemical formula for Acetic Acid ?</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>CH3COOH</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Which one of the given is commonly known as blue vitriol and is used as fungicide ?</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Potassium Nitrate, Copper Sulphate, Sodium Carbonate, Sodium Chloride</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Copper Sulphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Range of pH scale ?</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0 - 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Which one is different from others</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Nitric acid, Tartaric acid, Sulphuric acid, Phosphoric acid</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Tartaric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Common salt beside being used in the kitchen can also be used as the raw material for the production of
+A) Baking Powder
+B) Washing Soda
+C) Black Ash
+D) Slaked Lime</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(B) and (C), (A) and (C), (A) and (B), (B) and (D) </t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>(A) and (B)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>When electricity is passed through NaCl aqueous solution</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Sodium metal is deposited, Only chlorine gas is produced, Chlorine and Hydrogen gases are produce, All of the given are produced</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Chlorine and Hydrogen gases are produce</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vinegar is used in pickling as it</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Is an acid, Prevents the growth of microbes, Prevents drying of pickle, Increase taste</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Prevents the growth of microbes</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which of the following cannot be changed while balancing a chemical equation </t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>No of Atoms, No of Moleclues, Molecular formula, Molecular mass</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>No of Atoms</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating Tree Layout and Adding Subject DB Manager
</commit_message>
<xml_diff>
--- a/app/database/question_bank.xlsx
+++ b/app/database/question_bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,20 +476,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Columns in MS Excel are named in the form of ____</t>
+          <t>The neutralization reaction between an acid and a base is a type of</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BCE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>roman numerals, numbers, alphabets, none of them</t>
+          <t>Double displacement reaction, Displacement reaction, Addition reaction, Decomposition reaction</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -499,7 +497,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>alphabets</t>
+          <t>Double displacement reaction</t>
         </is>
       </c>
     </row>
@@ -509,20 +507,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rows in MS Excel are named in the form of ____</t>
+          <t>Which of the following gases is used in the storage of fat and oil-containing foods for long time?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BCE</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>alphabets, roman numerals, numbers, none of them</t>
+          <t>Carbon dioxide gas, Nitrogen gas, Oxygen gas, Neon gas</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -532,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>numbers</t>
+          <t>Nitrogen gas</t>
         </is>
       </c>
     </row>
@@ -542,12 +538,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The interaction of a row and column in MS Excel is called</t>
+          <t>When ferrous sulphate is heated strongly it undergoes decomposition to form ferric oxide as a main product accompanied by change in color form:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -555,7 +551,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>spreadsheet, workbook, document, cell</t>
+          <t>Blue to green, Green to blue, Green to brown, Green to yellow</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -565,7 +561,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>cell</t>
+          <t>Green to brown</t>
         </is>
       </c>
     </row>
@@ -575,12 +571,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>What is entered by the function =today() ?</t>
+          <t xml:space="preserve">All the methods mentioned below can be used to prevent the food from getting rancid except 
+i) Storing the food in the air-tight containers
+ii) Storing the food in refrigerator 
+iii) Keeping the food in clean and covering containers iv) Always touching the food with clean hands. </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -588,7 +587,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The date value for the day according to system clock, The time value according to system clock, Today's date as text format, All of Above</t>
+          <t>(i) and (ii), (i) and (iii), (i)(iii) and (iv), (iii) and (iv)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -598,7 +597,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>The date value for the day according to system clock</t>
+          <t>(iii) and (iv)</t>
         </is>
       </c>
     </row>
@@ -608,12 +607,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>In MS Excel, a function is entered by typing ___ symbol</t>
+          <t xml:space="preserve">It is necessary to balance a chemical equation in order to satisfy the law of </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -621,7 +620,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>@', '#', '=', '$'</t>
+          <t>Conservation of Motion, Conservation of mass, Conservation of momentum, Conservation of Energy</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -629,9 +628,10 @@
           <t>MCQ</t>
         </is>
       </c>
-      <c r="G6">
-        <f>'</f>
-        <v/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Conservation of mass</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -640,12 +640,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The latest version of MS Excel have ____ rows.</t>
+          <t>One of the following process does not involve a chemical reaction That is:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1048576, 16334, 102443, 5124</t>
+          <t>Melting of candle wax when heated, Burning of candle wax when heated, Digestion of food in our stomach, Ripening of Banana</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -661,8 +661,10 @@
           <t>MCQ</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>1048576</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Melting of candle wax when heated</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -671,12 +673,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The latest version of MS Excel have ____ columns.</t>
+          <t>A chemical reaction does not involve</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -684,7 +686,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>16384, 1048576, 5124, 102443</t>
+          <t>Formation of new substances having entirely different properties than that of the reactants, Breaking of old chemical bonds and formation of new chemical bonds, Rearrangement of the atoms of reactants to form new products, Changing of the atoms of one element into those of another element to form new products</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -692,8 +694,10 @@
           <t>MCQ</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>16384</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Changing of the atoms of one element into those of another element to form new products</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -702,25 +706,31 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Can you set a border for page layout in EXCEL ? (T/F)</t>
+          <t>The respiration process during which glucose undergoes slow combustion by combining with oxygen in the cells of our body to produce energy is a kind of:</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>2</v>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Exothermic Process, Endothermic Process, Reversible Process, Physical Process</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>True/False</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Exothermic Process</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -729,12 +739,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Each file in MS Excel is known as </t>
+          <t>In a chemical reaction between sulphuric acid and barium chloride solution the white precipitates formed are of:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -742,7 +752,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Notebook, worksheet, workbook, spreadsheet</t>
+          <t>Hydrochloric acid, Barium sulphate, Chlorine, Sulphur</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -752,7 +762,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>workbook</t>
+          <t>Barium sulphate</t>
         </is>
       </c>
     </row>
@@ -762,12 +772,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">By default excel worksheet are named as </t>
+          <t>Before burning in air, the magnesium ribbon is cleaned by rubbing with sandpaper to:</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -775,7 +785,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>book1..book2…book3, page1…page2…page3, sheet1…sheet2….sheet3, note1…note2…note3</t>
+          <t>Make the ribbon surface shiner, Remove the layer of magnesium oxide from the ribbon surface, Remove the layer of magnesium carbonate from the ribbon surface, Remove the moisture from the ribbon surface</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -785,7 +795,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>sheet1…sheet2….sheet3</t>
+          <t>Remove the layer of magnesium oxide from the ribbon surface</t>
         </is>
       </c>
     </row>
@@ -795,12 +805,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Which of the following is an absolute cell reference ?</t>
+          <t xml:space="preserve">Which of the following are exothermic processes?
+i) Reaction of water with quick lime 
+ii) Dilution of an acid
+iii) Evaporation of water
+iv) Submilation of crystals (camphor)  </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -808,7 +822,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>!A!1, $A$1, #a#1, A1</t>
+          <t>(i) and (ii), (ii) and (iii), (i) and (iv), (ii) and (iv)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -818,7 +832,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>$A$1</t>
+          <t>(i) and (ii)</t>
         </is>
       </c>
     </row>
@@ -828,29 +842,31 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Which symbol is used for all formula begin with ?</t>
+          <t>The process of reduction involves</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
-      <c r="E13">
-        <f>' '#', '@', ')'</f>
-        <v/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>addition of oxygen, addition of hydrogen, removal of hydrogen, removal of oxygen</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>MCQ</t>
         </is>
       </c>
-      <c r="G13">
-        <f>'</f>
-        <v/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>removal of oxygen</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -859,12 +875,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hyperlinks can be </t>
+          <t>A substance 'X' is used in white-whashing and is obtained by heating limestone in the absense of air. Identify 'X'.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>C01, Chemistry</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -872,7 +888,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Text, Drawings, Picture, All of Above</t>
+          <t>CaOCl2, Ca(OH)2, CaO, CaCo3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -882,7 +898,2127 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>CaO</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>What type of chemical reactions take place when electricity is passed through water?</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Displacement, Combination, Decomposition, Double Displacement</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Decomposition</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>A substance added to food containing fats and oils is called:</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Oxidant, Rancid, Coolant, Antioxidant</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Antioxidant</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Select the oxidising agent for the following reaction
+H2S + I2 -&gt; 2HI + S</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>I2, H2S, HI, S</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>I2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Which of the following is Not True with respect to the neutralization reaction?</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Salt is formed, Reaction occurs between an acid and a base, Reactive element displaces less reactive elements, Reactants are in gaseous state</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Reactants are in gaseous state</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Methyl orange is </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Pink in acidic medium and yellow in basic medium, Yellow in acidic medium and pink in basic medium, Colourless in acidic medium and pink in basic medium, Pink in acidic medium and colorless in basic medium</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Pink in acidic medium and yellow in basic medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lime water is </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CaO, Ca(OH)2, CaCo3, CaCl2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ca(OH)2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Which of the following salts has no water of crystallization ?</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Blue Vitrol, Washing Soda, Baking Soda, Gypsum</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Baking Soda</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Most of the oxides of metals when react with acid , form ___</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>A Base, An Acid, A Salt, Either (1) or (2)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>A Salt</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Generally, when certain metals react with an acid they release ___ gas.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Nitrogen, Oxygen, Hydrogen, Argon</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Which of the given is a strong base ?</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Calcium Hydroxide, Magnesium Hydroxide, Ammonium Hydroxide, Potassium Hydroxide</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Potassium Hydroxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Which one of the given is the PH value of pure water</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0, 7, 8, 1</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Which one of the following  is formed when calcium hydroxide reacts with carbon dioxide ?</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Hydrogen gas, Water, Salt, Both Water and Salt</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Both Water and Salt</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>When acids dissolve in water it releases ___.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>H+ ion, H- ion, H30+ ion, H302+ ion</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>H30+ ion</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Black ash is ___.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Dry KOH, Barium sulphate, Charcoal, Hydrated KOH</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Barium sulphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>The pH of commonly used toothpaste is ?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>&lt;6.5, ≥ 7, ≥ 2.2, None of these</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>≥ 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The pH of Gastric juice is </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>&lt;6.5, ≥ 7, 1.5 to 3.5, None of Above</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1.5 to 3.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>The chemical formula of Plaster of Paris is</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CaSo4, 1/2 H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>What happens when a solution of an acid is mixed with a solution of base in a test tube ?
+i) The temperature of the solution increases.
+ii) The temperature of the solution decreases.
+iii) The temperature of the solution remains the same.
+iv) Salt formation takes place.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>(i) only, (i) and (ii), (ii) and (iii), (i) and (iv)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>(i) and (iv)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chemical formula of washing soda is </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Na2Co3, 10H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>An aqueous solution turns red litmus solution blue. Excess addition of which of the following solution would be the reverse change ?</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Baking Powder, Lime, Ammonium hydroxide solution, Hydrochloric acid</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Hydrochloric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sodium Hydroxide is used </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>as an antacid, in manufacturing of soap, as a cleansing agent, in alkaline</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>in alkaline</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>The pH of a solution is 7. How can you increase its pH ?</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>By adding a small amount of acid, By adding small amount of base, By adding a small amount of salt, By passing carbon dioxide gas through it</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>By adding small amount of base</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Sodium hydroxide is a ____</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>weak base, weak acid, strong base, strong acid</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>strong base</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Which of the following gives the correct increasing order of acidic strength ?</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Water &lt; Acetic acid &lt; Hydrochloric acid, Water &lt; Hydrochloric acid &lt; Acetic acid, Acetic acid &lt; Water &lt; Hydrochloric acid, Hydrochloric acid &lt; Water &lt; Acetic acid</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Water &lt; Acetic acid &lt; Hydrochloric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Rain is called acid rain when its</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>pH falls below 7, pH falls below 6, pH falls below 5.6, pH is above 7</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>pH falls below 5.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>If a few drops of a concentrated acid accidentally spills over the hand of the student, what should be done ?</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Wash the hand with saline water, Wash the hand immediately with plenty of water and apply a paste of sodium hydrogencarbonate, After washing with plenty of water apply solution of sodium hydroxide on the hand., Neutralize the acid with a strong alkali</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Neutralize the acid with a strong alkali</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Farmers neutralize the effect of acidity of the soil by adding </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Slaked lime, gypsum, caustic soda, baking soda</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Slaked lime</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>What is the pH range of our body ?</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>7.0 - 7.8, 7.2 - 8.0, 7.0 - 8.4, 7.2 - 8.4</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>7.0 - 7.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Tooth enamel is made up of ?</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>calcium phosphate, calcium carbonate, calcium oxide, potassium</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>calcium phosphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Increase in the OH- ion concentration, leads to</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>an increase in the pH of solution, a decrease in the pH of solution, doesn't alter the pH of solution, decrease the basic strength of the solution.</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>an increase in the pH of solution</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Lime water reacts with chlorine to give</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>bleaching powder, baking powder, baking soda, washing soda</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>bleaching powder</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Alkalis are</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>acids (which are soluble in water), acids (which are insoluble in water), bases (which are soluble in water), bases (which are insoluble in water)</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>bases (which are soluble in water)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Acids react with metal carbonates to liberate ___ gas</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Carbon dioxide, Carbon monoxide, hydrogen, water</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Carbon monoxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Lime water turns milky when carbon dioxide is passed due to formation of ___.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>CaCO3, CaO, CO2, CaSo4</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>CaCO3</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How is the concentration of hydronium ions (H30+) affected when a solution of an acid is diluted </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Increases, Decreases, Remains same, Becomes Zero</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Decreases</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>From the following, which one is the example of chemical reaction ?</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Grapes get fermented, Breakdown of food, Formation of curd, All of the above</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>All of the above</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Which of the following shows an oxidation reaction ?</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Gain of Oxygen, Loss of Oxygen, Gain of Hydrogen, None of Above</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Gain of Oxygen</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>What is the product obtained when lead nitrate is heated ?</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Lead Oxide, Lead Nitrate, Lead Sulphate, Lead Chloride</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Lead Oxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>In a chemical equation, the number written in front of a chemical formula represents:</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Atomic Number, Molecular Mass, Number of Molecules, Number of atoms or molecules taking part in the reaction</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Number of Molecules</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>The balanced chemical equation for the reaction between hydrogen and oxygen to form water is:</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>H2 + O2 -&gt; H20, 2H2 + O2 -&gt; 2H20,  H20 -&gt; H2 + O2, 2H2O -&gt; 2H2 + O2</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2H2 + O2 -&gt; 2H20</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>The type of chemical reaction in which two or more substances combine to form a single product is called</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Combination Reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>What is the product obtained when copper (II) oxide is heated with hydrogen gas ?</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Copper Oxide, Copper Metal, Copper Sulphate, Copper Chloride</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Copper Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Which of the following statements is true regarding a decomposition reaction</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>A single reactant breaks down into two or more products, Two or more reactants combine to form a single product, A metal displaces another metal to form its salt solution, A non metal displaces another non-metal from its compound.</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>A single reactant breaks down into two or more products</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The chemical name of the baking soda commonly used in cooking is </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Sodium chloride, Sodium bicarbonate, Sodium carbonate, sodium hydroxide</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Sodium bicarbonate</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>The chemical formula for sulfuric acid is:</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>H2SO3, HCL, H2SO4, HNO3</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>H2SO4</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Reaction of 'magnesium' with air is</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Exothermic reaction, Endothermic reaction, Reversible reaction, Substitution</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Exothermic reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>What chemicals are used in fireworks</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Copper Chloride, Calcium Chloride, Barium Chloride, All of Above</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>All of Above</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>When crystals of lead nitrate are heated strongly in a dry test tube</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Crystals immediately melt, Brown residue is left, White fumes appear in the tube, A yellow residue is left</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Brown residue is left</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The reaction in which two compounds exchange their ions to form two new compounds is called </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Double displacement reaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Which of the following is characteristics of acids ?</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Sour Taste, Bitter Taste, Slippery feel, Blue litmus to Red</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Sour Taste</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Which of the following is a weak base ?</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Sodium hydroxide, Ammonium Hydroxide, Calcium Hydroxide, Potassium Hydroxide</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Ammonium Hydroxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Which of the following is an example of salt ?</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Sugar, Calcium Carbonate, Sodium Chloride, Hydrogen Peroxide</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Sodium Chloride</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>What is the chemical formula of hydrochloric acid is HCL ?</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>True/False</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Which of the following is natural indicator ?</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Phenolphthalein, Methyl Orange, Litmus, Vitrol Blue</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Litmus</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Which acid is found in vinegar ?</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Sulfuric Acid, Nitric Acid, Acetic Acid, HCL</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Acetic Acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>What is the pH value of lemon juice ?</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1, 7, 14, 5</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Which of the following is a weak acid ?</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>HCL, Sulfuric acid, Nitric Acid, Carbonic Acid</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Carbonic Acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>What is the chemical formula for Acetic Acid ?</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>CH3COOH</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Which one of the given is commonly known as blue vitriol and is used as fungicide ?</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Potassium Nitrate, Copper Sulphate, Sodium Carbonate, Sodium Chloride</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Copper Sulphate</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Range of pH scale ?</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0 - 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Which one is different from others</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Nitric acid, Tartaric acid, Sulphuric acid, Phosphoric acid</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Tartaric acid</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Common salt beside being used in the kitchen can also be used as the raw material for the production of
+A) Baking Powder
+B) Washing Soda
+C) Black Ash
+D) Slaked Lime</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(B) and (C), (A) and (C), (A) and (B), (B) and (D) </t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>(A) and (B)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>When electricity is passed through NaCl aqueous solution</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Sodium metal is deposited, Only chlorine gas is produced, Chlorine and Hydrogen gases are produce, All of the given are produced</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Chlorine and Hydrogen gases are produce</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vinegar is used in pickling as it</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>C02, Chemistry</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Is an acid, Prevents the growth of microbes, Prevents drying of pickle, Increase taste</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Prevents the growth of microbes</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which of the following cannot be changed while balancing a chemical equation </t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>C01, Chemistry</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>No of Atoms, No of Moleclues, Molecular formula, Molecular mass</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>No of Atoms</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Applying common fonts too all widgets
</commit_message>
<xml_diff>
--- a/app/database/question_bank.xlsx
+++ b/app/database/question_bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>L5CL2X</t>
+          <t>MQKJY9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Joule is unit of ______________ .</t>
+          <t>The reason for Sea Level rise is</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Work, Force, Time, Pressure</t>
+          <t>Depletion of ozone layer, Global warming, Smog, Acid Rain</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,24 +501,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Work</t>
+          <t>Global warming</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RD35YC</t>
+          <t>IMAG7Q</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Least count of Verneir Calipers is inversly proportional to</t>
+          <t>The type of generator used in HAWT which supply power to the grid line is</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Total division of Verneir scale, Coincident Mark, Length of main scale, Maximum range of Verneir Caliper</t>
+          <t>Synchronous Induction Generator, D.C Generator, A.C. Generator, Asynchronous Generator</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -536,24 +536,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Total division of Verneir scale</t>
+          <t>Synchronous Induction Generator</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>L3GV5O</t>
+          <t>JCHNCH</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yotta means</t>
+          <t>Atmosphere of big cities is polluted by</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -561,7 +561,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10²⁴, 10¹², 10⁹, 10⁶</t>
+          <t>Household Waste, Radioactive Fallout, Pesticides, Automobile Exhaust</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -571,24 +571,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>10²⁴</t>
+          <t>Automobile Exhaust</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PEDDCP</t>
+          <t>7LVESS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A vernier calipers has calibrated in mm and 19 of main scale division is equal to 20 division of vernier scale then L.C is</t>
+          <t>BOD Measures</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -596,7 +596,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.05 mm, 0.03 mm, 0.01 mm, 0.01 cm</t>
+          <t>content of bacteria, Content of inorganic matter, Carbonic matter in domestic sewage, OUD</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -606,24 +606,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.05 mm</t>
+          <t>Carbonic matter in domestic sewage</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OYDPEP</t>
+          <t>5BXZLR</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>How many significant figures are there in 9.4 × 10⁻¹⁰ ?</t>
+          <t>BOD stands for</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -631,7 +631,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4</t>
+          <t>Biochemical Oxygen Dissolution, Biochemical Oxygen Demand, Biochemical Oxidation Demand, Biological Oxygen Demand</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -641,24 +641,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Biochemical Oxygen Demand</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TSL4YW</t>
+          <t>77JGTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The prefix 'Giga' stands for _____.</t>
+          <t>The component of environment made of sea, rivers, lakes, etc is called</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10¹², 10³, 10⁶, 10⁹</t>
+          <t>Atmosphere, Hydrosphere, Biosphere, Lithosphere</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -676,24 +676,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10⁹</t>
+          <t>Hydrosphere</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BANV7M</t>
+          <t>5E3MPN</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The value of 6.02 × 10²³ represents _____.</t>
+          <t>In which atmospheric layer do most cloud form ?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Atomic Mass, Avagadro's number, Planck's constant, Speed of Light</t>
+          <t>Stratosphere, Atmosphere, Mesosphere, Troposphere</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -711,24 +711,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Avagadro's number</t>
+          <t>Troposphere</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Y2VY3U</t>
+          <t>DDBG0S</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>How many significant series are in 1.0070 ?</t>
+          <t>Which type of clouds are responible for thunderstorm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -736,7 +736,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1, 5, 4, 6</t>
+          <t>Cirrus, Stratus, Cumulonimbus, Nacreous</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -746,24 +746,24 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Cumulonimbus</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>53UNV6</t>
+          <t>H1O54A</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The smallest unit of length is ___________ .</t>
+          <t>Which is the lowest layer of the atmosphere</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -771,7 +771,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Centimeter, Micrometer, Millimeter, Nanometer</t>
+          <t>Stratosphere, Mesosphere, Troposphere, Thermosphere</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -781,24 +781,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Nanometer</t>
+          <t>Troposphere</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>U5XWIY</t>
+          <t>5UNR49</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Unit of surface tension is</t>
+          <t>The ozone layer is mainly found in which atmospheric layer</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N.m, m/N, Dyne/cm², J/m²</t>
+          <t>Troposphere, Stratosphere, Mesosphere, Exosphere</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -816,24 +816,24 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>J/m²</t>
+          <t>Stratosphere</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>XW3OFB</t>
+          <t>GW5AHZ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Which is fundamental quantity ?</t>
+          <t>In which layer do most airplanes fly ?</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Length, Voltage, Velocity, Voltage</t>
+          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -851,24 +851,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Length</t>
+          <t>Stratosphere</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6RAM6J</t>
+          <t>XYEDII</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1 dyne = _________ .</t>
+          <t>The hottest layer of the atmosphere is</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -876,7 +876,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>10⁻³ N, 10⁻⁵ N, 10⁻² N, 10⁻¹ N</t>
+          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -886,24 +886,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10⁻⁵ N</t>
+          <t>Thermosphere</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1DO0H6</t>
+          <t>C9CPQJ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Force is _____ .</t>
+          <t>Which layer is known as the "ionosphere" due to its charged particles ?</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Scalar Quantity, Fundamental Quantity, Vector Quantity, None of these</t>
+          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -921,24 +921,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Vector Quantity</t>
+          <t>Thermosphere</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CDDT92</t>
+          <t>6B454N</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Find out the force of an object having 20 g of mass and 20 cm/s of velocity.</t>
+          <t>The outermost layer of the Earth's atmosphere is called ?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -946,7 +946,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.02N, 0.2N, Cannot Be Determined, 2N</t>
+          <t>Troposphere, Mesosphere, Thermosphere, Exosphere</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Cannot Be Determined</t>
+          <t>Exosphere</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>9RBQUA</t>
+          <t>7VINIG</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>First law of Newton gives the definition of __________ .</t>
+          <t>In a food chain</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -981,7 +981,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Force, Inertia, Velocity, Weight</t>
+          <t>energy flows from tropic level-1 to tropic level-4, energy flows from tropic level-4 to tropic level-1, energy does not flow, energy flows from tropic level-4 to tropic level-3</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -991,24 +991,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Inertia</t>
+          <t>energy flows from tropic level-1 to tropic level-4</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HR8VR7</t>
+          <t>XHD9O5</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>According to Newton's First Law, the resistance offered by a body to change its state of motion is directly related to its __________.</t>
+          <t>Which fuel used in automobiles produce least pollution ?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Force, Velocity, Mass, Weight</t>
+          <t>CNG, LPG, Diesel, Petrol</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1026,24 +1026,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Mass</t>
+          <t>CNG</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SFIDRW</t>
+          <t>6MVMEP</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>If constant force applied on object then which quantity becomes constant</t>
+          <t>Coal is the main contributor of</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Speed, Power, Momentum, Acceleration</t>
+          <t>CO₂, SO₂, N₂, CO</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1061,24 +1061,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Acceleration</t>
+          <t>CO₂</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>O6EMZK</t>
+          <t>6WEZCY</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Inertia is ___________ .</t>
+          <t>Which gas is mainly responsible for green house effect ?</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>A property of matter, A type of force, The speed of an object, None of above</t>
+          <t>CO₂, CFC, CH₄, N₂O</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1096,24 +1096,24 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>A property of matter</t>
+          <t>CFC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>375Y1X</t>
+          <t>GJ72X7</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A and B are two objects with masses 1000 kg and 750 kg respectively, then</t>
+          <t>Hydrogen fuel cell</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Physcis</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Both will have same inertia, B will have more inertia, A will have more inertia, Both will have less inertia</t>
+          <t>produce electric power by burning of hydrogen gas, works like a battery, Does not require recharging, All of above</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1131,24 +1131,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>A will have more inertia</t>
+          <t>works like a battery</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AJ89IX</t>
+          <t>OG9JP0</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>The resultant balanced force is</t>
+          <t>What is typical number of blades in most mordern HAWTs ?</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Zero, Greater than Zero, Non Zero, Less than Zero</t>
+          <t>1, 2, 3, 6</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1166,24 +1166,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Zero</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5DYRSL</t>
+          <t>LM9WCS</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>When 1N force act on body of 1kg mass, the object moves with</t>
+          <t>What happens if the wind speed exceeds the turbine's cut-out speed ?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>A speed of 1m/s, A speed of 10m/s, Acceleration of 1m/s², Acceleration of 10m/s²</t>
+          <t>The turbine speeds up, The turbine stops to prevent damage, The turbine stores extra energy, The turbine reverses its rotation</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1201,24 +1201,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Acceleration of 1m/s²</t>
+          <t>The turbine stops to prevent damage</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AUOOS1</t>
+          <t>HVNHFE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The acceleration in a body due to</t>
+          <t>What is the main function of the yaw mechanism in a HAWT ?</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Unbalanced force, Balanced Force, Mass, Electrostatic Force</t>
+          <t>To adjust the blade pitch, To rotate the nacelle to face the wind, To slow down the rotor speed, To generate electricity directly</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1236,24 +1236,24 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Unbalanced force</t>
+          <t>To rotate the nacelle to face the wind</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4FDKBI</t>
+          <t>S79YZI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The physical quantity, which is equal to change in momentum is</t>
+          <t>Where are the most HAWTs installed ?</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Force, Acceleration, Velocity, Impulse</t>
+          <t>Underground, Offshore and Onshore, Inside buildings, In urban rooftops</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1271,24 +1271,24 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Impulse</t>
+          <t>Offshore and Onshore</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>N2GPDI</t>
+          <t>LIWGJX</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Momentum of a massive object at rest is</t>
+          <t>What is the main advantage of a HAWT over a VAWT (Vertical Axis Wind Turbine) ?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Very large, Zero, Very less, None of these</t>
+          <t>Can operate in all wind direction without orientation, More efficient at converting wind energy, Require less land area, Works better in low wind speed</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1306,24 +1306,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Zero</t>
+          <t>More efficient at converting wind energy</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>W1BF49</t>
+          <t>SGYA00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Unit of heat energy</t>
+          <t>In horizontal axis Wind Turbine (HAWT) where generator is placed ?</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Kelvin, Kilogram, Temperature, Joule</t>
+          <t>In the nessel, Above the tower, At ground level, In the gearbox</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1341,24 +1341,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Joule</t>
+          <t>In the nessel</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>V68EIE</t>
+          <t>73Y3YS</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bodies transmitting heat via radiation</t>
+          <t>Which of the following solid waste disposal methods is ecologically most acceptable ?</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Do not required medium, Need only solid medium, Need only liquid medium, Need only gaseous medium</t>
+          <t>Sanitary land fill, Inclineration, Composting, Pyrolysis</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1376,24 +1376,24 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Do not required medium</t>
+          <t>Composting</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>D2W0PZ</t>
+          <t>0T93V5</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>In Fahrenheit scale water freezes at</t>
+          <t>In a HAWT, the rotor shaft is aligned in which direction ?</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0 F, 40 F, 32 F, 212 F</t>
+          <t>Horizontal, Vertical, Diagonal, Perpendicular to wind Flow</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1411,24 +1411,24 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>212 F</t>
+          <t>Horizontal</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1QMWE8</t>
+          <t>ATY726</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>An iron ball at 40°C  is dropped in a mug containing water at 60°C. The heat will be</t>
+          <t>What does HAWT stand for ?</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Flow from iron ball to water, Increasing the temperature of both, Flow from water to ball, None of Above</t>
+          <t>Horizontal Axis Wind Turbine, Horizontal Axis Wind Tubeline, Horizonal Airflow wind Turbine, Hybrid Axis Wind Technology</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1446,24 +1446,24 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Flow from water to ball</t>
+          <t>Horizontal Axis Wind Turbine</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FONV54</t>
+          <t>B5U4YS</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The high thermal conductivity of metals is due to the free electrons. The relevant electron's Property is :</t>
+          <t>Which is the most common material used for mordern HAWT blades ?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Its Low Volume, Its low average thermal speed, Its being negatively charged, Its high average thermal speed</t>
+          <t>Carbon Fibre, Fibreglass - reinforced plastic, Pure aluminium, Titanium Alloy</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1481,24 +1481,24 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Its high average thermal speed</t>
+          <t>Fibreglass - reinforced plastic</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>B56UEP</t>
+          <t>72TN4D</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The quantity of heat flowing through a conductor is proportional to it :</t>
+          <t>The biggest pollutant receptor or sink on the earth is</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Cross sectional area, Temperature, Length, Coefficient of thermal expansion</t>
+          <t>Hyrdosphere, Lithosphere, Atmosphere, Biosphere</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1516,24 +1516,24 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Cross sectional area</t>
+          <t>Hyrdosphere</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>827ZJ7</t>
+          <t>9CRL27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>The amount of heat in calories required to heat 2 kg of water from 20°C to 80°C is :</t>
+          <t>As per IS Code, the acceptable noise level in urban residental area is</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>120, 12 × 10⁶, 12 × 10⁴, 12 × 10²</t>
+          <t>35-45 dBA, 45-55 dBA, 30-40 dBA, 40-50 dBA</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1551,24 +1551,24 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>12 × 10⁴</t>
+          <t>35-45 dBA</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PVZ43I</t>
+          <t>Q3A4ZG</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The temperature of a body is 90° C. Its temperature is Fahrenheit is given by :-</t>
+          <t>Which is the largest ecosystem on the earth ?</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>19.4, 164, 123, 194</t>
+          <t>Forests, Sea, Deserts, Grasslands</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1586,24 +1586,24 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>Sea</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>WT1ZRU</t>
+          <t>IUQBES</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Which of the following is a unit of heat capacity?</t>
+          <t>In biogas plant, digestion takes place in the absense of</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>J°C⁻¹, J·kg⁻¹·°C⁻¹, J·kg⁻¹, None of these</t>
+          <t>Oxygen, Carbon dioxide, Hydrogen, Methane</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1621,24 +1621,24 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>J°C⁻¹</t>
+          <t>Oxygen</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>9QGC5T</t>
+          <t>SGY0BX</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The wavelength of sound in air is 10 cm. its frequency is, (Given velocity of sound = 330 m/s)</t>
+          <t>The daily cover of MSW landfills consists of which of the following</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>330 cycles per second, 3.3 kilo cycles per second, 30 mega-cycles per second, 3 × 10⁵ cycles per second</t>
+          <t>Compacted Soil, Geomembrane, Geotextile, Geocomposite</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1656,24 +1656,24 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>3.3 kilo cycles per second</t>
+          <t>Compacted Soil</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P1XXLH</t>
+          <t>ADHUWA</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>In the longitudinal waves the direction of vibration in medium of particle is</t>
+          <t>In the atmosphere reaction between Nitrogen oxides, hydrocarbon and sunlight produces</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Perpendicular to propagation of wave, Parallel to propagation, Different from each other, Variable for time to time</t>
+          <t>Sulphur Dioxide, Benzene, CO, PAN</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1691,24 +1691,24 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Parallel to propagation</t>
+          <t>PAN</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0RB3WI</t>
+          <t>WUAHUD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Which of the following correctly represents the relation between velocity (v), frequency (f), and wavelength (λ)?</t>
+          <t>Noise pollution is measured in</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>v = f / λ, f = v × λ, λ = v / f, v = λ / f</t>
+          <t>Decibel, Newton, Dyne, ECO</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1726,24 +1726,24 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>λ = v / f</t>
+          <t>Decibel</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>FMBJLJ</t>
+          <t>Z7NVHM</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>With the propagation of a longitudinal wave through a material medium the quantities transmitted in the propagation direction is</t>
+          <t>Vegetables, grass, trees, etc are which type of biotic components ?</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Energy, momentum and mass, Energy, Energy and Mass, Energy and Linear Momentum</t>
+          <t>Producers, Consumers, Decomposers, Transformers</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1761,24 +1761,24 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Energy and Linear Momentum</t>
+          <t>Producers</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>QRAGUP</t>
+          <t>R8YXIP</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The velocity of sound is maximum in</t>
+          <t>Nacelle is used in</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Water, Vacuum, Air, Metal</t>
+          <t>Darious wind turbine, Savonious wind turbine, Horizontal axis wind turbine, Water pumping wind mill</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1796,24 +1796,24 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>Horizontal axis wind turbine</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>V1YGKC</t>
+          <t>932EXG</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>In the wave equation y = 0.25 sin(310t), the value 0.25 represents :</t>
+          <t>Due to 'Ozone hole' in the earth's atmosphere, which ray comes to earth surface ?</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Frequency, Amplitude, Wavelength, Phase</t>
+          <t>Laser rays, X-rays, Ultravoilet rays, None of these</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1831,24 +1831,24 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Amplitude</t>
+          <t>Ultravoilet rays</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>HFU9L4</t>
+          <t>MP134F</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>The velocity of sound in vacuum is</t>
+          <t>Less of removal of the superficial layer of soil by the action of water, wind, or by the human activites are termed as</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Zero, 341 m/s, 330 m/s, 440 m/s</t>
+          <t>Soil Erosion, Soil Pollution, Desertification, Salination</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1866,24 +1866,24 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Zero</t>
+          <t>Soil Erosion</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>WMKNOK</t>
+          <t>OYAT71</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Which is not simple harmonic motion?</t>
+          <t>Minamata disease is caused by ____</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Motion of projectile, Motion of swing, Motion of simple pendulum, Motion of atom</t>
+          <t>Mercury, Lead, Zinc, Manganese</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Motion of projectile</t>
+          <t>Mercury</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>RFKH3C</t>
+          <t>27WJIU</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A sound wave travels from air to water, which of following quantities remain unchanged</t>
+          <t>Which of the following is an artifical ecosystem ?</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Frequency, Intensity, Wavelength, Velocity</t>
+          <t>Forests, Desert, Fish house, Pond</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1936,24 +1936,24 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t>Fish house</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ERITNP</t>
+          <t>XVPYOI</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The relation between intensity (I) and amplitude (A) of waves is:</t>
+          <t>Which pollutant is primarily responsible for causing respiratory problems and cardiovascular diseases in humans ?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>I ∝ A, I ∝ 1/A, I ∝ A², I ∝ 1/A²</t>
+          <t>Lead, Benzene, Carbon Monoxide (CO), Particulate matter (PM10)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1971,24 +1971,24 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>I ∝ A²</t>
+          <t>Particulate matter (PM10)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>OYAZJS</t>
+          <t>WH53C3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Frequency of ultrasonic waves is</t>
+          <t>What is the approximately range of mordern solar photovoltaic (PV) panels in converting sunlight in to electricity ?</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>More than 20Hz, More than 2000Hz, More than 200Hz, More than 20000Hz</t>
+          <t>5-10%, 15-20%, 20-30%, 40-50%</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2006,24 +2006,24 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>More than 20000Hz</t>
+          <t>15-20%</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ZLF63F</t>
+          <t>1MI8GU</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The pitch of sound waves measured by</t>
+          <t>CFCs are not recommended to be used in refridgerator because they ____</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Loudness, Frequency, Gas, Sharpness</t>
+          <t>Increase Temperature, Deplete Ozone, Affect Environment, Affect Human Body</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2041,24 +2041,24 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t>Deplete Ozone</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CZGDQH</t>
+          <t>F4FMI3</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Snell's Rule is</t>
+          <t>Clouds are present ____ in layer of atmosphere.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>sin r / sin i = n₁ / n₂, n₁ × tan i = n₂ × tan r, sin i = sin r, n₁ × sin i = n₂ × sin r</t>
+          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2076,24 +2076,24 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>n₁ × sin i = n₂ × sin r</t>
+          <t>Troposphere</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>96HZDX</t>
+          <t>KKDLYR</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The ratio of image size and object size is defined by</t>
+          <t>Which pollutant is commonly associated with blue baby syndrome in infants ?</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Largeness, Diopter, Magnification, Center of length</t>
+          <t>Lead, Arsenic, Mercury, Nitrate</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2111,24 +2111,24 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Magnification</t>
+          <t>Nitrate</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>R7ZHPL</t>
+          <t>UWO0O6</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>If a force is applied to an object, the length of the object changes. This is an example of:</t>
+          <t>Which disease is known as 'pain-pain-diseases' due to serve bone pain and fractures ?</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Elastic collision, Deformation, Thermal expansion, Translational motion</t>
+          <t>Black Lung Disease, Itai-Itai Disease, Sillicosis, Fluorosis</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2146,24 +2146,24 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Deformation</t>
+          <t>Itai-Itai Disease</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>E2EAWK</t>
+          <t>C2T882</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>If a force is applied to an object, the length of the object changes. This is an example of:</t>
+          <t>Which occupational diseases is caused by inhaling coal dust over a long period ?</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Newton's Second Law, Snell's Law, Hooke's Law, Pascal's Law</t>
+          <t>Asbestosis, Silicosis, Black Lung Diseases, Eutrophication</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2181,24 +2181,24 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Hooke's Law</t>
+          <t>Black Lung Diseases</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PY6IEG</t>
+          <t>65P9UL</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Viscosity is a property of:</t>
+          <t>What is the primary poltant responsivle for Flurosis ?</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Solid, Liquid, Gas, Plasma</t>
+          <t>Fluroide, Lead, Sulfur dioxide, Arsenic</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2216,7 +2216,147 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Liquid</t>
+          <t>Fluroide</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>IAI21L</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>The BHOPAL GAS TRAGEDY was caused due to which leakage of gas ?</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Carbon Monoxide, Methyl isocyanate (MIC), Sulfur dioxide, Nitrogen dioxide</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Methyl isocyanate (MIC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>481PMN</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Which disease is associated with inhaling silica dust ?</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Silicosis, Asbestosis, Itai-Itai Disease, Blue Baby Syndrome</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Silicosis</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>S2UOWF</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Acid Rain is mainly caused by which pollutants ?</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Carbon monoxide and Lead, Nitrogen oxide and Sulphur dioxide, Fluoride and Mercury, Ozone and PM2.5</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Nitrogen oxide and Sulphur dioxide</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ALJDJ9</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>What is the main source of Cadmium Contamination leading to Itai-Itai diseases</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Fertilizer runoff, Industrial wastewater, burning of fossil fuels, Oil spills</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Industrial wastewater</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improvising UI [PDF Generation] [Cloud Export]
</commit_message>
<xml_diff>
--- a/app/database/question_bank.xlsx
+++ b/app/database/question_bank.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,19 +471,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>MQKJY9</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The reason for Sea Level rise is</t>
+          <t>Full form of CPU is ____</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -491,34 +489,32 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Depletion of ozone layer, Global warming, Smog, Acid Rain</t>
+          <t>Central Processing Unit, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Global warming</t>
+          <t>Central Processing Unit</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>IMAG7Q</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The type of generator used in HAWT which supply power to the grid line is</t>
+          <t>Full form of RAM is ____</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -526,34 +522,32 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Synchronous Induction Generator, D.C Generator, A.C. Generator, Asynchronous Generator</t>
+          <t>Random Access Memory, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Synchronous Induction Generator</t>
+          <t>Random Access Memory</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>JCHNCH</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Atmosphere of big cities is polluted by</t>
+          <t>Full form of ROM is ____</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -561,34 +555,32 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Household Waste, Radioactive Fallout, Pesticides, Automobile Exhaust</t>
+          <t>Read Only Memory, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Automobile Exhaust</t>
+          <t>Read Only Memory</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>7LVESS</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BOD Measures</t>
+          <t>Full form of USB is ____</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -596,34 +588,32 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>content of bacteria, Content of inorganic matter, Carbonic matter in domestic sewage, OUD</t>
+          <t>Universal Serial Bus, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Carbonic matter in domestic sewage</t>
+          <t>Universal Serial Bus</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5BXZLR</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOD stands for</t>
+          <t>Full form of CD is ____</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -631,34 +621,32 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Biochemical Oxygen Dissolution, Biochemical Oxygen Demand, Biochemical Oxidation Demand, Biological Oxygen Demand</t>
+          <t>Compact Disc, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Biochemical Oxygen Demand</t>
+          <t>Compact Disc</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>77JGTD</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The component of environment made of sea, rivers, lakes, etc is called</t>
+          <t>Full form of DVD is ____</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -666,34 +654,32 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Atmosphere, Hydrosphere, Biosphere, Lithosphere</t>
+          <t>Digital Versatile Disc, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hydrosphere</t>
+          <t>Digital Versatile Disc</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>5E3MPN</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>In which atmospheric layer do most cloud form ?</t>
+          <t>Full form of LED is ____</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -701,34 +687,32 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Stratosphere, Atmosphere, Mesosphere, Troposphere</t>
+          <t>Light Emitting Diode, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Troposphere</t>
+          <t>Light Emitting Diode</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>DDBG0S</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Which type of clouds are responible for thunderstorm</t>
+          <t>Full form of LCD is ____</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -736,34 +720,32 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Cirrus, Stratus, Cumulonimbus, Nacreous</t>
+          <t>Liquid Crystal Display, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Cumulonimbus</t>
+          <t>Liquid Crystal Display</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>H1O54A</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Which is the lowest layer of the atmosphere</t>
+          <t>Full form of UPS is ____</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -771,34 +753,32 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Stratosphere, Mesosphere, Troposphere, Thermosphere</t>
+          <t>Uninterruptible Power Supply, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Troposphere</t>
+          <t>Uninterruptible Power Supply</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>5UNR49</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The ozone layer is mainly found in which atmospheric layer</t>
+          <t>Full form of OS is ____</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -806,34 +786,32 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Mesosphere, Exosphere</t>
+          <t>Operating System, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Stratosphere</t>
+          <t>Operating System</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>GW5AHZ</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>In which layer do most airplanes fly ?</t>
+          <t>Full form of PC is ____</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -841,34 +819,32 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
+          <t>Personal Computer, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Stratosphere</t>
+          <t>Personal Computer</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>XYEDII</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The hottest layer of the atmosphere is</t>
+          <t>Full form of GPU is ____</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -876,34 +852,32 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
+          <t>Graphics Processing Unit, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Thermosphere</t>
+          <t>Graphics Processing Unit</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>C9CPQJ</t>
-        </is>
+      <c r="A14" t="n">
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Which layer is known as the "ionosphere" due to its charged particles ?</t>
+          <t>Full form of IP is ____</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -911,34 +885,32 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
+          <t>Internet Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Thermosphere</t>
+          <t>Internet Protocol</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>6B454N</t>
-        </is>
+      <c r="A15" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The outermost layer of the Earth's atmosphere is called ?</t>
+          <t>Full form of URL is ____</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -946,34 +918,32 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Troposphere, Mesosphere, Thermosphere, Exosphere</t>
+          <t>Uniform Resource Locator, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Exosphere</t>
+          <t>Uniform Resource Locator</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>7VINIG</t>
-        </is>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>In a food chain</t>
+          <t>Full form of HTTP is ____</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -981,34 +951,32 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>energy flows from tropic level-1 to tropic level-4, energy flows from tropic level-4 to tropic level-1, energy does not flow, energy flows from tropic level-4 to tropic level-3</t>
+          <t>HyperText Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>energy flows from tropic level-1 to tropic level-4</t>
+          <t>HyperText Transfer Protocol</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>XHD9O5</t>
-        </is>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Which fuel used in automobiles produce least pollution ?</t>
+          <t>Full form of HTTPS is ____</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1016,34 +984,32 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CNG, LPG, Diesel, Petrol</t>
+          <t>HyperText Transfer Protocol Secure, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>CNG</t>
+          <t>HyperText Transfer Protocol Secure</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>6MVMEP</t>
-        </is>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Coal is the main contributor of</t>
+          <t>Full form of WWW is ____</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1051,34 +1017,32 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CO₂, SO₂, N₂, CO</t>
+          <t>World Wide Web, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>CO₂</t>
+          <t>World Wide Web</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>6WEZCY</t>
-        </is>
+      <c r="A19" t="n">
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Which gas is mainly responsible for green house effect ?</t>
+          <t>Full form of ISP is ____</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1086,34 +1050,32 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CO₂, CFC, CH₄, N₂O</t>
+          <t>Internet Service Provider, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>Internet Service Provider</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>GJ72X7</t>
-        </is>
+      <c r="A20" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hydrogen fuel cell</t>
+          <t>Full form of LAN is ____</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1121,34 +1083,32 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>produce electric power by burning of hydrogen gas, works like a battery, Does not require recharging, All of above</t>
+          <t>Local Area Network, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>works like a battery</t>
+          <t>Local Area Network</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>OG9JP0</t>
-        </is>
+      <c r="A21" t="n">
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>What is typical number of blades in most mordern HAWTs ?</t>
+          <t>Full form of WAN is ____</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1156,34 +1116,32 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1, 2, 3, 6</t>
+          <t>Wide Area Network, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Wide Area Network</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LM9WCS</t>
-        </is>
+      <c r="A22" t="n">
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>What happens if the wind speed exceeds the turbine's cut-out speed ?</t>
+          <t>Full form of VPN is ____</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1191,34 +1149,32 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The turbine speeds up, The turbine stops to prevent damage, The turbine stores extra energy, The turbine reverses its rotation</t>
+          <t>Virtual Private Network, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The turbine stops to prevent damage</t>
+          <t>Virtual Private Network</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>HVNHFE</t>
-        </is>
+      <c r="A23" t="n">
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>What is the main function of the yaw mechanism in a HAWT ?</t>
+          <t>Full form of DNS is ____</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1226,34 +1182,32 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>To adjust the blade pitch, To rotate the nacelle to face the wind, To slow down the rotor speed, To generate electricity directly</t>
+          <t>Domain Name System, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>To rotate the nacelle to face the wind</t>
+          <t>Domain Name System</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>S79YZI</t>
-        </is>
+      <c r="A24" t="n">
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Where are the most HAWTs installed ?</t>
+          <t>Full form of MAC is ____</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1261,34 +1215,32 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Underground, Offshore and Onshore, Inside buildings, In urban rooftops</t>
+          <t>Media Access Control, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Offshore and Onshore</t>
+          <t>Media Access Control</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>LIWGJX</t>
-        </is>
+      <c r="A25" t="n">
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>What is the main advantage of a HAWT over a VAWT (Vertical Axis Wind Turbine) ?</t>
+          <t>Full form of GUI is ____</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1296,34 +1248,32 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Can operate in all wind direction without orientation, More efficient at converting wind energy, Require less land area, Works better in low wind speed</t>
+          <t>Graphical User Interface, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>More efficient at converting wind energy</t>
+          <t>Graphical User Interface</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>SGYA00</t>
-        </is>
+      <c r="A26" t="n">
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>In horizontal axis Wind Turbine (HAWT) where generator is placed ?</t>
+          <t>Full form of API is ____</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1331,34 +1281,32 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>In the nessel, Above the tower, At ground level, In the gearbox</t>
+          <t>Application Programming Interface, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>In the nessel</t>
+          <t>Application Programming Interface</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>73Y3YS</t>
-        </is>
+      <c r="A27" t="n">
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Which of the following solid waste disposal methods is ecologically most acceptable ?</t>
+          <t>Full form of IDE is ____</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1366,34 +1314,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Sanitary land fill, Inclineration, Composting, Pyrolysis</t>
+          <t>Integrated Development Environment, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Composting</t>
+          <t>Integrated Development Environment</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>0T93V5</t>
-        </is>
+      <c r="A28" t="n">
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>In a HAWT, the rotor shaft is aligned in which direction ?</t>
+          <t>Full form of SQL is ____</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1401,34 +1347,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Horizontal, Vertical, Diagonal, Perpendicular to wind Flow</t>
+          <t>Structured Query Language, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Horizontal</t>
+          <t>Structured Query Language</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>ATY726</t>
-        </is>
+      <c r="A29" t="n">
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>What does HAWT stand for ?</t>
+          <t>Full form of HTML is ____</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1436,34 +1380,32 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Horizontal Axis Wind Turbine, Horizontal Axis Wind Tubeline, Horizonal Airflow wind Turbine, Hybrid Axis Wind Technology</t>
+          <t>HyperText Markup Language, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Horizontal Axis Wind Turbine</t>
+          <t>HyperText Markup Language</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>B5U4YS</t>
-        </is>
+      <c r="A30" t="n">
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Which is the most common material used for mordern HAWT blades ?</t>
+          <t>Full form of CSS is ____</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1471,34 +1413,32 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Carbon Fibre, Fibreglass - reinforced plastic, Pure aluminium, Titanium Alloy</t>
+          <t>Cascading Style Sheets, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Fibreglass - reinforced plastic</t>
+          <t>Cascading Style Sheets</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>72TN4D</t>
-        </is>
+      <c r="A31" t="n">
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The biggest pollutant receptor or sink on the earth is</t>
+          <t>Full form of XML is ____</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1506,34 +1446,32 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hyrdosphere, Lithosphere, Atmosphere, Biosphere</t>
+          <t>eXtensible Markup Language, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Hyrdosphere</t>
+          <t>eXtensible Markup Language</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>9CRL27</t>
-        </is>
+      <c r="A32" t="n">
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>As per IS Code, the acceptable noise level in urban residental area is</t>
+          <t>Full form of JSON is ____</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1541,34 +1479,32 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>35-45 dBA, 45-55 dBA, 30-40 dBA, 40-50 dBA</t>
+          <t>JavaScript Object Notation, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>35-45 dBA</t>
+          <t>JavaScript Object Notation</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Q3A4ZG</t>
-        </is>
+      <c r="A33" t="n">
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Which is the largest ecosystem on the earth ?</t>
+          <t>Full form of PHP is ____</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1576,34 +1512,32 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Forests, Sea, Deserts, Grasslands</t>
+          <t>Hypertext Preprocessor, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Sea</t>
+          <t>Hypertext Preprocessor</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>IUQBES</t>
-        </is>
+      <c r="A34" t="n">
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>In biogas plant, digestion takes place in the absense of</t>
+          <t>Full form of AI is ____</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1611,34 +1545,32 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Oxygen, Carbon dioxide, Hydrogen, Methane</t>
+          <t>Artificial Intelligence, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Oxygen</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>SGY0BX</t>
-        </is>
+      <c r="A35" t="n">
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The daily cover of MSW landfills consists of which of the following</t>
+          <t>Full form of SSD is ____</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1646,34 +1578,32 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Compacted Soil, Geomembrane, Geotextile, Geocomposite</t>
+          <t>Solid State Drive, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Compacted Soil</t>
+          <t>Solid State Drive</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>ADHUWA</t>
-        </is>
+      <c r="A36" t="n">
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>In the atmosphere reaction between Nitrogen oxides, hydrocarbon and sunlight produces</t>
+          <t>Full form of HDD is ____</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1681,34 +1611,32 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Sulphur Dioxide, Benzene, CO, PAN</t>
+          <t>Hard Disk Drive, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>Hard Disk Drive</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>WUAHUD</t>
-        </is>
+      <c r="A37" t="n">
+        <v>36</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Noise pollution is measured in</t>
+          <t>Full form of BIOS is ____</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1716,34 +1644,32 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Decibel, Newton, Dyne, ECO</t>
+          <t>Basic Input Output System, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Decibel</t>
+          <t>Basic Input Output System</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Z7NVHM</t>
-        </is>
+      <c r="A38" t="n">
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vegetables, grass, trees, etc are which type of biotic components ?</t>
+          <t>Full form of PDF is ____</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1751,34 +1677,32 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Producers, Consumers, Decomposers, Transformers</t>
+          <t>Portable Document Format, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Producers</t>
+          <t>Portable Document Format</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>R8YXIP</t>
-        </is>
+      <c r="A39" t="n">
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nacelle is used in</t>
+          <t>Full form of ZIP is ____</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1786,34 +1710,32 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Darious wind turbine, Savonious wind turbine, Horizontal axis wind turbine, Water pumping wind mill</t>
+          <t>Zone Improvement Plan, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Horizontal axis wind turbine</t>
+          <t>Zone Improvement Plan</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>932EXG</t>
-        </is>
+      <c r="A40" t="n">
+        <v>39</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Due to 'Ozone hole' in the earth's atmosphere, which ray comes to earth surface ?</t>
+          <t>Full form of GNU is ____</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1821,34 +1743,32 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Laser rays, X-rays, Ultravoilet rays, None of these</t>
+          <t>GNU's Not Unix, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ultravoilet rays</t>
+          <t>GNU's Not Unix</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>MP134F</t>
-        </is>
+      <c r="A41" t="n">
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Less of removal of the superficial layer of soil by the action of water, wind, or by the human activites are termed as</t>
+          <t>Full form of TOR is ____</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1856,34 +1776,32 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Soil Erosion, Soil Pollution, Desertification, Salination</t>
+          <t>The Onion Router, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Soil Erosion</t>
+          <t>The Onion Router</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>OYAT71</t>
-        </is>
+      <c r="A42" t="n">
+        <v>41</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Minamata disease is caused by ____</t>
+          <t>Full form of SSH is ____</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1891,34 +1809,32 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Mercury, Lead, Zinc, Manganese</t>
+          <t>Secure Shell, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>Secure Shell</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>27WJIU</t>
-        </is>
+      <c r="A43" t="n">
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Which of the following is an artifical ecosystem ?</t>
+          <t>Full form of SMTP is ____</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1926,34 +1842,32 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Forests, Desert, Fish house, Pond</t>
+          <t>Simple Mail Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Fish house</t>
+          <t>Simple Mail Transfer Protocol</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>XVPYOI</t>
-        </is>
+      <c r="A44" t="n">
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Which pollutant is primarily responsible for causing respiratory problems and cardiovascular diseases in humans ?</t>
+          <t>Full form of POP3 is ____</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1961,34 +1875,32 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Lead, Benzene, Carbon Monoxide (CO), Particulate matter (PM10)</t>
+          <t>Post Office Protocol version 3, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Particulate matter (PM10)</t>
+          <t>Post Office Protocol version 3</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>WH53C3</t>
-        </is>
+      <c r="A45" t="n">
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>What is the approximately range of mordern solar photovoltaic (PV) panels in converting sunlight in to electricity ?</t>
+          <t>Full form of IMAP is ____</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1996,34 +1908,32 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5-10%, 15-20%, 20-30%, 40-50%</t>
+          <t>Internet Message Access Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>15-20%</t>
+          <t>Internet Message Access Protocol</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>1MI8GU</t>
-        </is>
+      <c r="A46" t="n">
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CFCs are not recommended to be used in refridgerator because they ____</t>
+          <t>Full form of DHCP is ____</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -2031,34 +1941,32 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Increase Temperature, Deplete Ozone, Affect Environment, Affect Human Body</t>
+          <t>Dynamic Host Configuration Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Deplete Ozone</t>
+          <t>Dynamic Host Configuration Protocol</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>F4FMI3</t>
-        </is>
+      <c r="A47" t="n">
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Clouds are present ____ in layer of atmosphere.</t>
+          <t>Full form of RAID is ____</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2066,34 +1974,32 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
+          <t>Redundant Array of Independent Disks, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Troposphere</t>
+          <t>Redundant Array of Independent Disks</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>KKDLYR</t>
-        </is>
+      <c r="A48" t="n">
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Which pollutant is commonly associated with blue baby syndrome in infants ?</t>
+          <t>Full form of TFTP is ____</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -2101,34 +2007,32 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Lead, Arsenic, Mercury, Nitrate</t>
+          <t>Trivial File Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Nitrate</t>
+          <t>Trivial File Transfer Protocol</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>UWO0O6</t>
-        </is>
+      <c r="A49" t="n">
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Which disease is known as 'pain-pain-diseases' due to serve bone pain and fractures ?</t>
+          <t>Full form of DSL is ____</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2136,34 +2040,32 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Black Lung Disease, Itai-Itai Disease, Sillicosis, Fluorosis</t>
+          <t>Digital Subscriber Line, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Itai-Itai Disease</t>
+          <t>Digital Subscriber Line</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>C2T882</t>
-        </is>
+      <c r="A50" t="n">
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Which occupational diseases is caused by inhaling coal dust over a long period ?</t>
+          <t>Full form of CAPTCHA is ____</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2171,34 +2073,32 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Asbestosis, Silicosis, Black Lung Diseases, Eutrophication</t>
+          <t>Completely Automated Public Turing test to tell Computers and Humans Apart, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Black Lung Diseases</t>
+          <t>Completely Automated Public Turing test to tell Computers and Humans Apart</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>65P9UL</t>
-        </is>
+      <c r="A51" t="n">
+        <v>50</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>What is the primary poltant responsivle for Flurosis ?</t>
+          <t>Full form of MODEM is ____</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -2206,34 +2106,32 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Fluroide, Lead, Sulfur dioxide, Arsenic</t>
+          <t>Modulator-Demodulator, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Fluroide</t>
+          <t>Modulator-Demodulator</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>IAI21L</t>
-        </is>
+      <c r="A52" t="n">
+        <v>51</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The BHOPAL GAS TRAGEDY was caused due to which leakage of gas ?</t>
+          <t>Full form of NIC is ____</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -2241,34 +2139,32 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Carbon Monoxide, Methyl isocyanate (MIC), Sulfur dioxide, Nitrogen dioxide</t>
+          <t>Network Interface Card, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Methyl isocyanate (MIC)</t>
+          <t>Network Interface Card</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>481PMN</t>
-        </is>
+      <c r="A53" t="n">
+        <v>52</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Which disease is associated with inhaling silica dust ?</t>
+          <t>Full form of IP is ____</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -2276,34 +2172,32 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Silicosis, Asbestosis, Itai-Itai Disease, Blue Baby Syndrome</t>
+          <t>Internet Protocol, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Silicosis</t>
+          <t>Internet Protocol</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>S2UOWF</t>
-        </is>
+      <c r="A54" t="n">
+        <v>53</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Acid Rain is mainly caused by which pollutants ?</t>
+          <t>Full form of URL is ____</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -2311,34 +2205,32 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Carbon monoxide and Lead, Nitrogen oxide and Sulphur dioxide, Fluoride and Mercury, Ozone and PM2.5</t>
+          <t>Uniform Resource Locator, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Nitrogen oxide and Sulphur dioxide</t>
+          <t>Uniform Resource Locator</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>ALJDJ9</t>
-        </is>
+      <c r="A55" t="n">
+        <v>54</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>What is the main source of Cadmium Contamination leading to Itai-Itai diseases</t>
+          <t>Full form of HTML is ____</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>C10, Computer</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -2346,17 +2238,1535 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Fertilizer runoff, Industrial wastewater, burning of fossil fuels, Oil spills</t>
+          <t>HyperText Markup Language, Wrong1, Wrong2, Wrong3</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>MCQ</t>
+          <t>One Word</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Industrial wastewater</t>
+          <t>HyperText Markup Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Full form of CSS is ____</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Cascading Style Sheets, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Cascading Style Sheets</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Full form of JS is ____</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>JavaScript, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>JavaScript</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Full form of AJAX is ____</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Asynchronous JavaScript and XML, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Asynchronous JavaScript and XML</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Full form of SQL is ____</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Structured Query Language, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Structured Query Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Full form of DBMS is ____</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Database Management System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Database Management System</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Full form of RDBMS is ____</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Relational Database Management System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Relational Database Management System</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Full form of BIOS is ____</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Basic Input Output System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Basic Input Output System</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Full form of HTTP is ____</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>HyperText Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>HyperText Transfer Protocol</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Full form of HTTPS is ____</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>HyperText Transfer Protocol Secure, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>HyperText Transfer Protocol Secure</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Full form of FTP is ____</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>File Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>File Transfer Protocol</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Full form of SMTP is ____</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>2</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Simple Mail Transfer Protocol, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Simple Mail Transfer Protocol</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Full form of POP3 is ____</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Post Office Protocol version 3, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Post Office Protocol version 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Full form of IMAP is ____</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Internet Message Access Protocol, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Internet Message Access Protocol</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Full form of LAN is ____</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Local Area Network, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Local Area Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Full form of WAN is ____</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Wide Area Network, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Wide Area Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Full form of MAN is ____</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Metropolitan Area Network, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Metropolitan Area Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Full form of PAN is ____</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Personal Area Network, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Personal Area Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Full form of ISP is ____</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Internet Service Provider, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Internet Service Provider</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Full form of VOIP is ____</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Voice Over Internet Protocol, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Voice Over Internet Protocol</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Full form of MAC is ____</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Media Access Control, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Media Access Control</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Full form of IPTV is ____</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Internet Protocol Television, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Internet Protocol Television</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Full form of VPN is ____</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Virtual Private Network, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Virtual Private Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Full form of DOS is ____</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>2</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Disk Operating System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Disk Operating System</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Full form of OS is ____</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Operating System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Operating System</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Full form of GUI is ____</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>2</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Graphical User Interface, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Graphical User Interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Full form of CLI is ____</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>2</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Command Line Interface, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Command Line Interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Full form of AI is ____</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>2</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Full form of ML is ____</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>2</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Machine Learning, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Full form of IOT is ____</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>2</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Internet of Things, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Internet of Things</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Full form of PDF is ____</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>2</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Portable Document Format, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Portable Document Format</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Full form of PNG is ____</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>2</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Portable Network Graphics, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Portable Network Graphics</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Full form of JPEG is ____</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>2</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Joint Photographic Experts Group, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Joint Photographic Experts Group</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Full form of GIF is ____</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>2</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Graphics Interchange Format, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Graphics Interchange Format</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Full form of MP3 is ____</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>2</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>MPEG Audio Layer 3, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>MPEG Audio Layer 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Full form of MP4 is ____</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>2</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>MPEG-4 Part 14, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>MPEG-4 Part 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Full form of WIFI is ____</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>2</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Wireless Fidelity, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Wireless Fidelity</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Full form of GPS is ____</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Global Positioning System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Global Positioning System</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Full form of SSD is ____</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Solid State Drive, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Solid State Drive</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Full form of HDD is ____</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Hard Disk Drive, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Hard Disk Drive</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Full form of CAD is ____</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>2</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Computer Aided Design, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Computer Aided Design</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Full form of CAM is ____</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Computer Aided Manufacturing, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Computer Aided Manufacturing</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Full form of CRT is ____</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>2</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Cathode Ray Tube, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Cathode Ray Tube</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Full form of SMPS is ____</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Switched Mode Power Supply, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Switched Mode Power Supply</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Full form of DSL is ____</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Digital Subscriber Line, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Digital Subscriber Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Full form of IoS is ____</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>iPhone Operating System, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>iPhone Operating System</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Full form of OEM is ____</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>C10, Computer</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Original Equipment Manufacturer, Wrong1, Wrong2, Wrong3</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>One Word</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Original Equipment Manufacturer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalizing according to client requirements
</commit_message>
<xml_diff>
--- a/app/database/question_bank.xlsx
+++ b/app/database/question_bank.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQKJY9</t>
+          <t>99O3K3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The reason for Sea Level rise is</t>
+          <t>Which of the following are the primary cause of water pollution ?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Depletion of ozone layer, Global warming, Smog, Acid Rain</t>
+          <t>Plants, Animals, Human Activites, None of These</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,19 +501,19 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Global warming</t>
+          <t>Human Activites</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMAG7Q</t>
+          <t>3OWLVO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The type of generator used in HAWT which supply power to the grid line is</t>
+          <t>Which of the following is a non-renewable energy resource ?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Synchronous Induction Generator, D.C Generator, A.C. Generator, Asynchronous Generator</t>
+          <t>solar, methane, Hydroelectric, coal</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -536,19 +536,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Synchronous Induction Generator</t>
+          <t>coal</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>JCHNCH</t>
+          <t>DQ47WH</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Atmosphere of big cities is polluted by</t>
+          <t>Gardens are examples of</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Household Waste, Radioactive Fallout, Pesticides, Automobile Exhaust</t>
+          <t>Natural Ecosystem, Artificial Ecosystem, Ecological, Environment</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -571,19 +571,19 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Automobile Exhaust</t>
+          <t>Artificial Ecosystem</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7LVESS</t>
+          <t>9B8KER</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BOD Measures</t>
+          <t>Which of the following is the indirect use of forests ?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>content of bacteria, Content of inorganic matter, Carbonic matter in domestic sewage, OUD</t>
+          <t>Medical Plants, Checking Soil Erosion, Building Material, Grazing</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -606,19 +606,19 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Carbonic matter in domestic sewage</t>
+          <t>Checking Soil Erosion</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5BXZLR</t>
+          <t>YJ7V4O</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOD stands for</t>
+          <t>Which one of the following is an aquatic ecosystem ?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Biochemical Oxygen Dissolution, Biochemical Oxygen Demand, Biochemical Oxidation Demand, Biological Oxygen Demand</t>
+          <t>WetLand, Desert, Island, Mountain</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -641,19 +641,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Biochemical Oxygen Demand</t>
+          <t>WetLand</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>77JGTD</t>
+          <t>DPNS1Y</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The component of environment made of sea, rivers, lakes, etc is called</t>
+          <t>Which pollutant is commonly associated with "blue baby Syndrome" is infants ?</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Atmosphere, Hydrosphere, Biosphere, Lithosphere</t>
+          <t>Lead, Arsenic, Mercury, Nitrate</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -676,19 +676,19 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hydrosphere</t>
+          <t>Nitrate</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5E3MPN</t>
+          <t>PWQ090</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>In which atmospheric layer do most cloud form ?</t>
+          <t>Clouds are present in _____ layer of atmosphere.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Stratosphere, Atmosphere, Mesosphere, Troposphere</t>
+          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -718,12 +718,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DDBG0S</t>
+          <t>OGFW80</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Which type of clouds are responible for thunderstorm</t>
+          <t>CFCs are not recommended to be used in refrigerators because they _________</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Cirrus, Stratus, Cumulonimbus, Nacreous</t>
+          <t>Increase Temperature, Affect Environment, Deplete Ozone, Affect Human Body</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -746,19 +746,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Cumulonimbus</t>
+          <t>Deplete Ozone</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>H1O54A</t>
+          <t>ILQGZ6</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Which is the lowest layer of the atmosphere</t>
+          <t>What is the approximate effeciency range of modern solar photovoltaic (PV) panels in converting sunlight to electricity ?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Stratosphere, Mesosphere, Troposphere, Thermosphere</t>
+          <t>5-10%, 15-20%, 20-30%, 40-50%</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -781,19 +781,19 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Troposphere</t>
+          <t>15-20%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5UNR49</t>
+          <t>O9WN6F</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The ozone layer is mainly found in which atmospheric layer</t>
+          <t>Which pollutant is primarily responsible for causing respiratory problems and cardiovascular diseases in humans ?</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Mesosphere, Exosphere</t>
+          <t>Lead, Benzene, Particulate Matter (PM10), Carbon Monoxide</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -816,19 +816,19 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Stratosphere</t>
+          <t>Particulate Matter (PM10)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GW5AHZ</t>
+          <t>7JT7EG</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>In which layer do most airplanes fly ?</t>
+          <t>The component of environment made of sea, river, lake etc is called _______ .</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
+          <t>Hydrosphere, Lithosphere, Biosphere, Atmosphere</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -851,19 +851,19 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Stratosphere</t>
+          <t>Hydrosphere</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>XYEDII</t>
+          <t>8LYCVX</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The hottest layer of the atmosphere is</t>
+          <t>Which of the following is biodegradable pollutant ?</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
+          <t>Plastic, Domestic Sewage, Detergent, All of these</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -886,19 +886,19 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Thermosphere</t>
+          <t>Domestic Sewage</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C9CPQJ</t>
+          <t>GHMVWK</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Which layer is known as the "ionosphere" due to its charged particles ?</t>
+          <t>The Taj Mahal being affected by _______ .</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Troposphere, Stratosphere, Thermosphere, Mesosphere</t>
+          <t>Air Pollution, Water Pollution, Noise Pollution, None of Above</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -921,19 +921,19 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Thermosphere</t>
+          <t>Air Pollution</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>6B454N</t>
+          <t>9RYRXX</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The outermost layer of the Earth's atmosphere is called ?</t>
+          <t>The absorber plate of solar heater is made of _______.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Troposphere, Mesosphere, Thermosphere, Exosphere</t>
+          <t>Glass, Iron, Timber, Plastic</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -956,19 +956,19 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Exosphere</t>
+          <t>Iron</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>7VINIG</t>
+          <t>7ARTMB</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>In a food chain</t>
+          <t>Lithosphere consist of</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>energy flows from tropic level-1 to tropic level-4, energy flows from tropic level-4 to tropic level-1, energy does not flow, energy flows from tropic level-4 to tropic level-3</t>
+          <t>Water, Forest, Land, None of these</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -991,19 +991,19 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>energy flows from tropic level-1 to tropic level-4</t>
+          <t>Land</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>XHD9O5</t>
+          <t>HP1G8M</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Which fuel used in automobiles produce least pollution ?</t>
+          <t>Which is the component of Environment ?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CNG, LPG, Diesel, Petrol</t>
+          <t>Water, Animal, Land, All of these</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1026,19 +1026,19 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>CNG</t>
+          <t>All of these</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6MVMEP</t>
+          <t>RWZJA6</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Coal is the main contributor of</t>
+          <t>Blades of HAWT have</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CO₂, SO₂, N₂, CO</t>
+          <t>Aerospace design, Aerodynamic design, Aerometer design, All of them</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1061,19 +1061,19 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>CO₂</t>
+          <t>Aerodynamic design</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6WEZCY</t>
+          <t>GEULO0</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Which gas is mainly responsible for green house effect ?</t>
+          <t>Cutting of trees will</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CO₂, CFC, CH₄, N₂O</t>
+          <t>increase oxygen, increase carbon dioxide, increase ammonia, reduce carbon dioxide</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1096,19 +1096,19 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>increase carbon dioxide</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GJ72X7</t>
+          <t>COMDOD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hydrogen fuel cell</t>
+          <t>Energy auditing is done to</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>produce electric power by burning of hydrogen gas, works like a battery, Does not require recharging, All of above</t>
+          <t>Increasing energy use, Reduce energy use, Waste energy, A, B and C</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1131,19 +1131,19 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>works like a battery</t>
+          <t>Reduce energy use</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OG9JP0</t>
+          <t>73S6L4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>What is typical number of blades in most mordern HAWTs ?</t>
+          <t>Which place is famous for solar park in Gujarat ?</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1, 2, 3, 6</t>
+          <t>Surat, Charanka, Baroda, Harij</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1166,19 +1166,19 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Charanka</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LM9WCS</t>
+          <t>2RCEXE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>What happens if the wind speed exceeds the turbine's cut-out speed ?</t>
+          <t>Which of the following belongs to the category of primary consumers ?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The turbine speeds up, The turbine stops to prevent damage, The turbine stores extra energy, The turbine reverses its rotation</t>
+          <t>Snakes and Frog, Insects and Cattle, Eagle and Snakes, Water insects</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1201,19 +1201,19 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The turbine stops to prevent damage</t>
+          <t>Insects and Cattle</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>HVNHFE</t>
+          <t>CFM5WC</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>What is the main function of the yaw mechanism in a HAWT ?</t>
+          <t>Solar cell is made of ________ .</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>To adjust the blade pitch, To rotate the nacelle to face the wind, To slow down the rotor speed, To generate electricity directly</t>
+          <t>Conductor, Semi-Transistor, Transistor, Semi-Conductor</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1236,19 +1236,19 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>To rotate the nacelle to face the wind</t>
+          <t>Semi-Conductor</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>S79YZI</t>
+          <t>E6BPZP</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Where are the most HAWTs installed ?</t>
+          <t>_______ energy is an inexhaustible non conventional universal source of energy.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Underground, Offshore and Onshore, Inside buildings, In urban rooftops</t>
+          <t>Wind, Solar, Tidal, Hydrothermal</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1271,19 +1271,19 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Offshore and Onshore</t>
+          <t>Solar</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LIWGJX</t>
+          <t>CIAA2K</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>What is the main advantage of a HAWT over a VAWT (Vertical Axis Wind Turbine) ?</t>
+          <t>The study of earthquake and related effect is called ______ .</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Can operate in all wind direction without orientation, More efficient at converting wind energy, Require less land area, Works better in low wind speed</t>
+          <t>Seismology, Geology, Anatomy, Biology</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1306,19 +1306,19 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>More efficient at converting wind energy</t>
+          <t>Seismology</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SGYA00</t>
+          <t>O927EP</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>In horizontal axis Wind Turbine (HAWT) where generator is placed ?</t>
+          <t>Fuel formed under the earth's surface by the decomposition of organic matter is called ____.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>In the nessel, Above the tower, At ground level, In the gearbox</t>
+          <t>Organic fuel, Biogas, Fossil Fuel, Underground Fuel</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1341,19 +1341,19 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>In the nessel</t>
+          <t>Fossil Fuel</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>73Y3YS</t>
+          <t>L5P90J</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Which of the following solid waste disposal methods is ecologically most acceptable ?</t>
+          <t>Which gas in highest proportions in the constituents of bio gas ?</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Sanitary land fill, Inclineration, Composting, Pyrolysis</t>
+          <t>Nitrogen, Oxygen, Carbon, Methane</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1376,19 +1376,19 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Composting</t>
+          <t>Methane</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0T93V5</t>
+          <t>HGTJR5</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>In a HAWT, the rotor shaft is aligned in which direction ?</t>
+          <t>Example of natural disaster is _______ .</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Horizontal, Vertical, Diagonal, Perpendicular to wind Flow</t>
+          <t>Cyclone, Riots, Curfew, None of Above</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1411,19 +1411,19 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Horizontal</t>
+          <t>Cyclone</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ATY726</t>
+          <t>0RHRYB</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>What does HAWT stand for ?</t>
+          <t>What is the main source for the formation of wind ?</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Horizontal Axis Wind Turbine, Horizontal Axis Wind Tubeline, Horizonal Airflow wind Turbine, Hybrid Axis Wind Technology</t>
+          <t>Uneven Land, Sun, Vegetation, Seasons</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1446,19 +1446,19 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Horizontal Axis Wind Turbine</t>
+          <t>Sun</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>B5U4YS</t>
+          <t>DYX0K6</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Which is the most common material used for mordern HAWT blades ?</t>
+          <t>Wind generator is used for _______ .</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Carbon Fibre, Fibreglass - reinforced plastic, Pure aluminium, Titanium Alloy</t>
+          <t>Heat generation, Hydro plant, Power generation, Power consumption</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1481,19 +1481,19 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Fibreglass - reinforced plastic</t>
+          <t>Power generation</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>72TN4D</t>
+          <t>20XXMM</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The biggest pollutant receptor or sink on the earth is</t>
+          <t>Both power and manure is provided by _______.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hyrdosphere, Lithosphere, Atmosphere, Biosphere</t>
+          <t>Biogas plant, Thermal Plant, Solar Plant, Hydroplant</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1516,19 +1516,19 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Hyrdosphere</t>
+          <t>Biogas plant</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>9CRL27</t>
+          <t>EU1G8J</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>As per IS Code, the acceptable noise level in urban residental area is</t>
+          <t>Waste heat recovery is possible in ________.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>35-45 dBA, 45-55 dBA, 30-40 dBA, 40-50 dBA</t>
+          <t>Bus, Train, Boiler, None of Above</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1551,19 +1551,19 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>35-45 dBA</t>
+          <t>Boiler</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q3A4ZG</t>
+          <t>4NDJMS</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Which is the largest ecosystem on the earth ?</t>
+          <t>P and S waves are related to _______ .</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Forests, Sea, Deserts, Grasslands</t>
+          <t>Earthquake, Hurricane, Tsunami, Fire</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1586,19 +1586,19 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Sea</t>
+          <t>Earthquake</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>IUQBES</t>
+          <t>XREJU7</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>In biogas plant, digestion takes place in the absense of</t>
+          <t>_____ can be used to measure ozone in the stratosphere from the ground.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Oxygen, Carbon dioxide, Hydrogen, Methane</t>
+          <t>Spectrometer, Photometer, Spectrophoto meter, None of Above</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1621,19 +1621,19 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Oxygen</t>
+          <t>Spectrometer</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SGY0BX</t>
+          <t>KHHB8A</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The daily cover of MSW landfills consists of which of the following</t>
+          <t>The scattered solar radiation is called ________ radiation.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Compacted Soil, Geomembrane, Geotextile, Geocomposite</t>
+          <t>Direct, Beam, Diffused, Infrared</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1656,19 +1656,19 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Compacted Soil</t>
+          <t>Diffused</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ADHUWA</t>
+          <t>56DNX8</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>In the atmosphere reaction between Nitrogen oxides, hydrocarbon and sunlight produces</t>
+          <t>Another name for Earthquakes is _________ .</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Sulphur Dioxide, Benzene, CO, PAN</t>
+          <t>Nektons, Temblors, Blusters, Flickers</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1691,19 +1691,19 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>Temblors</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>WUAHUD</t>
+          <t>12LX5I</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Noise pollution is measured in</t>
+          <t>Man made earthquake can take place due to _________ .</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Decibel, Newton, Dyne, ECO</t>
+          <t>By celestial body, By atomic test, By volcanic activity, None of Above</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1726,19 +1726,19 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Decibel</t>
+          <t>By atomic test</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Z7NVHM</t>
+          <t>BS1S1C</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vegetables, grass, trees, etc are which type of biotic components ?</t>
+          <t>Which one is not a pollutant normally ?</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Producers, Consumers, Decomposers, Transformers</t>
+          <t>Hydrocarbon, Carbon Dioxide, Carbon Monoxide, Sulphur Dioxide</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1761,19 +1761,19 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Producers</t>
+          <t>Carbon Dioxide</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R8YXIP</t>
+          <t>OMEJ5L</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nacelle is used in</t>
+          <t>Major aerosol pollutant in jet plane emmision is _________ .</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Darious wind turbine, Savonious wind turbine, Horizontal axis wind turbine, Water pumping wind mill</t>
+          <t>Flurocarbon, Carbon Monoxide, Sulphur Dioxide, Methane</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1796,19 +1796,19 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Horizontal axis wind turbine</t>
+          <t>Flurocarbon</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>932EXG</t>
+          <t>BW6C0A</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Due to 'Ozone hole' in the earth's atmosphere, which ray comes to earth surface ?</t>
+          <t>Pyramid of numbers in tree ecosystem is __________ .</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Laser rays, X-rays, Ultravoilet rays, None of these</t>
+          <t>Always inverted, Always upright, Both of the above, None of the above</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1831,19 +1831,19 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ultravoilet rays</t>
+          <t>None of the above</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MP134F</t>
+          <t>2TUMT6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Less of removal of the superficial layer of soil by the action of water, wind, or by the human activites are termed as</t>
+          <t>Which of the following is the most stable ecosystem ?</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Soil Erosion, Soil Pollution, Desertification, Salination</t>
+          <t>Mountain, Ocean, Forest, Dessert</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1866,19 +1866,19 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Soil Erosion</t>
+          <t>Ocean</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>OYAT71</t>
+          <t>7Y7L3Q</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Minamata disease is caused by ____</t>
+          <t>What is the main function of wind wane ?</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Mercury, Lead, Zinc, Manganese</t>
+          <t>To measure wind velocity, To indicate wind direction, To measure wind energy, To indicate wind temperature</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1901,19 +1901,19 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Mercury</t>
+          <t>To indicate wind direction</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>27WJIU</t>
+          <t>ORD27O</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Which of the following is an artifical ecosystem ?</t>
+          <t>TDS is term related with ________.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Forests, Desert, Fish house, Pond</t>
+          <t>Water, Air, Gas, Solid waste</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1936,19 +1936,19 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Fish house</t>
+          <t>Water</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>XVPYOI</t>
+          <t>8ZH809</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Which pollutant is primarily responsible for causing respiratory problems and cardiovascular diseases in humans ?</t>
+          <t>Which state have highest wind power installed capacity ?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Lead, Benzene, Carbon Monoxide (CO), Particulate matter (PM10)</t>
+          <t>Tamil Nadu, Maharstra, Haryana, Gujarat</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1971,19 +1971,19 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Particulate matter (PM10)</t>
+          <t>Gujarat</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>WH53C3</t>
+          <t>OARFIE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>What is the approximately range of mordern solar photovoltaic (PV) panels in converting sunlight in to electricity ?</t>
+          <t>Biodiversity Act of India was passed by the parliament in the year</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5-10%, 15-20%, 20-30%, 40-50%</t>
+          <t>1992, 1990, 2000, 2002</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2006,19 +2006,19 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>15-20%</t>
+          <t>2002</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1MI8GU</t>
+          <t>8E73TB</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CFCs are not recommended to be used in refridgerator because they ____</t>
+          <t>Which of the following is not the type of biomass ?</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Increase Temperature, Deplete Ozone, Affect Environment, Affect Human Body</t>
+          <t>Bio diesel, Plastic, Dry Leaves, Agro Waste</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2041,19 +2041,19 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Deplete Ozone</t>
+          <t>Plastic</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>F4FMI3</t>
+          <t>CJVYR7</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Clouds are present ____ in layer of atmosphere.</t>
+          <t>A buffer stock of grains and grass useful during which period ?</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Stratosphere, Troposphere, Thermosphere, Mesosphere</t>
+          <t>Summer, Winter, Famines and Draughts, Monsoon</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2076,19 +2076,19 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Troposphere</t>
+          <t>Famines and Draughts</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>KKDLYR</t>
+          <t>SMGZJS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Which pollutant is commonly associated with blue baby syndrome in infants ?</t>
+          <t>Corona Virus is an example of _______.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Lead, Arsenic, Mercury, Nitrate</t>
+          <t>Pandemic, Pollutant, Cyclone, None of Above</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2111,19 +2111,19 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Nitrate</t>
+          <t>Pandemic</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>UWO0O6</t>
+          <t>QAJDOY</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Which disease is known as 'pain-pain-diseases' due to serve bone pain and fractures ?</t>
+          <t>When was the term 'Sustainable Development' came into existence ?</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Black Lung Disease, Itai-Itai Disease, Sillicosis, Fluorosis</t>
+          <t>2000, 1980, 2015, 1992</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2146,19 +2146,19 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Itai-Itai Disease</t>
+          <t>1980</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>C2T882</t>
+          <t>871VYM</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Which occupational diseases is caused by inhaling coal dust over a long period ?</t>
+          <t>Food web is network of interconnected  ___________.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Asbestosis, Silicosis, Black Lung Diseases, Eutrophication</t>
+          <t>Food Chain, Chain Web, Web Cycle, Ecosystem</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2181,19 +2181,19 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Black Lung Diseases</t>
+          <t>Food Chain</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>65P9UL</t>
+          <t>7OZ1DK</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>What is the primary poltant responsivle for Flurosis ?</t>
+          <t>In which part do we fnd sensors and actuators ?</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Fluroide, Lead, Sulfur dioxide, Arsenic</t>
+          <t>Gear, Turbine, Blades, Control System</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2216,19 +2216,19 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Fluroide</t>
+          <t>Control System</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>IAI21L</t>
+          <t>BX8886</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The BHOPAL GAS TRAGEDY was caused due to which leakage of gas ?</t>
+          <t>The example of renewable source of energy is _______ .</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Carbon Monoxide, Methyl isocyanate (MIC), Sulfur dioxide, Nitrogen dioxide</t>
+          <t>LPG, CNG, PNG, Tidal Energy</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2251,19 +2251,19 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Methyl isocyanate (MIC)</t>
+          <t>Tidal Energy</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>481PMN</t>
+          <t>W1ZDG4</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Which disease is associated with inhaling silica dust ?</t>
+          <t>Tremors experienced after major earthquake are called as _________.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Silicosis, Asbestosis, Itai-Itai Disease, Blue Baby Syndrome</t>
+          <t>Foreshocks, P-Waves, Aftershocks, S-Waves</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2286,19 +2286,19 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Silicosis</t>
+          <t>Aftershocks</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>S2UOWF</t>
+          <t>LN165U</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Acid Rain is mainly caused by which pollutants ?</t>
+          <t>Vertical axis wind turbine is</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Carbon monoxide and Lead, Nitrogen oxide and Sulphur dioxide, Fluoride and Mercury, Ozone and PM2.5</t>
+          <t>American Multiblade, Propeller Type, Savonious Type, None of These</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2321,19 +2321,19 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Nitrogen oxide and Sulphur dioxide</t>
+          <t>Savonious Type</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ALJDJ9</t>
+          <t>3501L2</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>What is the main source of Cadmium Contamination leading to Itai-Itai diseases</t>
+          <t>Which is not the type of pollution ?</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Fertilizer runoff, Industrial wastewater, burning of fossil fuels, Oil spills</t>
+          <t>Thermal Pollution, Eyes Pollution, Radioactive pollution, Land Pollution</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2356,7 +2356,217 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Industrial wastewater</t>
+          <t>Eyes Pollution</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>P9UG98</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Screening, Focculation, Sedimentation are related to ______ .</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Treatment of air, Treatment of water, Treatment of land, Treatment of noise</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Treatment of water</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>4QJ0MO</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Which of the following is an artificial ecosystem ?</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Fish House, Space Station, Farm, All of Above</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>All of Above</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>QU2N2T</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Energy auditing is done to ___________.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Increase Energy, Reduce Energy, Waste Energy, A, B and C</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Reduce Energy</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>0Z6NMS</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>By which process charcoal is made ?</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Anaerobic process, Hydrolysis, Pyrolysis, Biochemical process</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Pyrolysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ERVZGB</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Which plate is to be used to absorb heat containing in solar radiation ?</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Reducer, Absorber, Reflector, Rejector</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Absorber</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>7Y5DTD</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Which of the following is not a natural resource ?</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Forest, Plastic, Minerals, Water</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>MCQ</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Plastic</t>
         </is>
       </c>
     </row>

</xml_diff>